<commit_message>
ajout au plan de test pour la page d'horaire
</commit_message>
<xml_diff>
--- a/Tests/Plan_de_test.xlsx
+++ b/Tests/Plan_de_test.xlsx
@@ -1,44 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CEGEP\Hiver_2024\PRO\SPU\Tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE9C200-BCF0-4B07-A9AB-D7DD890B7D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
+    <workbookView xWindow="28680" yWindow="-7755" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Horaire" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Utilisateur" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Évaluations" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Chat" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Horaire" sheetId="1" r:id="rId1"/>
+    <sheet name="Utilisateur" sheetId="2" r:id="rId2"/>
+    <sheet name="Évaluations" sheetId="3" r:id="rId3"/>
+    <sheet name="Chat" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="126">
   <si>
     <t>Tests</t>
   </si>
   <si>
-    <t xml:space="preserve">Résultats attendus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Résultat obtenu</t>
+    <t>Résultats attendus</t>
+  </si>
+  <si>
+    <t>Résultat obtenu</t>
   </si>
   <si>
     <t>Commentaires</t>
   </si>
   <si>
-    <t xml:space="preserve">Supprimer une plage horaire.</t>
+    <t>Supprimer une plage horaire.</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">La plage horaire de l</t>
+      <t>La plage horaire de l</t>
     </r>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Aptos Narrow"/>
@@ -57,311 +64,387 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Ajouter une seule plage horaire qui est déjà prise.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Message d'erreur, retour à modifier plage horaire.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ajouter une récurrence de plage horaire mais une des plages horaires est déjà prises.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ajouter une date de fin est inférieur à la date de début.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ajouter une plage horaire de plus de 24 heures.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ajouter plage horaire déjà existante pour l'horaire en cours.</t>
+    <t>Ajouter une seule plage horaire qui est déjà prise.</t>
+  </si>
+  <si>
+    <t>Message d'erreur, retour à modifier plage horaire.</t>
+  </si>
+  <si>
+    <t>Ajouter une récurrence de plage horaire mais une des plages horaires est déjà prises.</t>
+  </si>
+  <si>
+    <t>Ajouter une date de fin est inférieur à la date de début.</t>
+  </si>
+  <si>
+    <t>Ajouter une plage horaire de plus de 24 heures.</t>
+  </si>
+  <si>
+    <t>Ajouter plage horaire déjà existante pour l'horaire en cours.</t>
   </si>
   <si>
     <t xml:space="preserve">Impossible d'ajouter la plage horaire. </t>
   </si>
   <si>
-    <t xml:space="preserve">Se connecter, stagiaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Redirection vers la page d'accueil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Redirection vers la page d'accueil avec succès</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se connecter, coordonateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Redirection vers la page de gestion des utilisateurs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Redirection vers la page de gestion des utilisateurs avec succès</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se connecter, maître de stage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se connecter, employeur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Redirection vers la page de gestion des maîtres de stages</t>
+    <t>Se connecter, stagiaire</t>
+  </si>
+  <si>
+    <t>Redirection vers la page d'accueil</t>
+  </si>
+  <si>
+    <t>Redirection vers la page d'accueil avec succès</t>
+  </si>
+  <si>
+    <t>Se connecter, coordonateur</t>
+  </si>
+  <si>
+    <t>Redirection vers la page de gestion des utilisateurs</t>
+  </si>
+  <si>
+    <t>Redirection vers la page de gestion des utilisateurs avec succès</t>
+  </si>
+  <si>
+    <t>Se connecter, maître de stage</t>
+  </si>
+  <si>
+    <t>Se connecter, employeur</t>
+  </si>
+  <si>
+    <t>Redirection vers la page de gestion des maîtres de stages</t>
   </si>
   <si>
     <t>Échec</t>
   </si>
   <si>
-    <t xml:space="preserve">Pas encore implémentée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se connecter, enseignant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entrer les bonnes données de connexion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accès à l'application</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accès à l'application avec succès</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Afficher des messages d'erreurs lorsque informations de connexion incorrectes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Échec de connexion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Échec avec succès</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accès restreint lorsqu'on est pas connecté</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reste sur la page de connexion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reste sur la page de connexion avec succès</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bouton se souvenir de moi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pas besoin de remplir à chaque fois ses identifiants</t>
+    <t>Pas encore implémentée</t>
+  </si>
+  <si>
+    <t>Se connecter, enseignant</t>
+  </si>
+  <si>
+    <t>Entrer les bonnes données de connexion</t>
+  </si>
+  <si>
+    <t>Accès à l'application</t>
+  </si>
+  <si>
+    <t>Accès à l'application avec succès</t>
+  </si>
+  <si>
+    <t>Afficher des messages d'erreurs lorsque informations de connexion incorrectes</t>
+  </si>
+  <si>
+    <t>Échec de connexion</t>
+  </si>
+  <si>
+    <t>Échec avec succès</t>
+  </si>
+  <si>
+    <t>Accès restreint lorsqu'on est pas connecté</t>
+  </si>
+  <si>
+    <t>Reste sur la page de connexion</t>
+  </si>
+  <si>
+    <t>Reste sur la page de connexion avec succès</t>
+  </si>
+  <si>
+    <t>Bouton se souvenir de moi</t>
+  </si>
+  <si>
+    <t>Pas besoin de remplir à chaque fois ses identifiants</t>
   </si>
   <si>
     <t>Succès</t>
   </si>
   <si>
-    <t xml:space="preserve">Se déconnecter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Être déconnecté</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stagiaires n'a accès qu'aux pages qui lui sont permises</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accès refusé s'il essaie d'accéder à une page à laquelle il n'a pas droit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accès refusé avec succès</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enseignant n'a accès qu'aux pages qui lui sont permises</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maître de stage n'a accès qu'aux pages qui lui sont permises</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employeur n'a accès qu'aux pages qui lui sont permises</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordonateur crée chaque utilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utilisateur crée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avec succès</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordonateur associe les utilisateurs à des rôles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rôles associés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordonateur peut modifier chaque utilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utilisateur modifié</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordonateur peut supprimer chaque utilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utilisateur supprimé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordonateur peut relier ensemble enseignant et stagiaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stagiaires-Enseignants associés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordonateur peut relier ensemble maître de stage s'il y a enseignant et stagiaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maitre de stage associés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordonateur peut modifier la liaison entre maître de stage et stagiaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liaison modifiée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordonateur peut modifier la liaison entre enseignant et stagiaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordonateur a accès à la page de gestion des utilisateurs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liste des utilisateurs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordonateur peut fournir des liens de connexion aux utilisateurs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liens copiés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pas encore implementé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validation des champs de formulaires</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Informations validées</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementé, mais pas partout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordonateur: accéder à la page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aucun accès</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enseignant: accéder à la page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Table de toutes les évaluations du prof est affichée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MDS et stagiaire: accéder à la page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seulement les évaluations liées au user ET active sont affichées</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enseignant: ajouter une évaluation active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L'évaluation est créée et chaque instance est active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enseignant: ajouter une évaluation non active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L'évaluation est créée et chaque instance n'est pas active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enseignant: ajouter une évaluation pour les mds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tout les mds liées aux étudiants de l'enseignant ont une évaluation créée pour eux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enseignant: ajouter une évaluation pour les stagiaires</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tout les étudiants de l'enseignant ont une évaluation créée pour eux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enseignant: Supprimer une évaluation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Toutes les évaluations en lien avec ce lien sont supprimées</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enseignant: changer l'activité d'une évaluation pour un utilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le nouveau status de l'évaluation est enregistré</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Étudiant ou MDS: clicker sur un lien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le status "consulté" de l'évaluation est mis à jour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le lien est ouvert dans le browser de l'utilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accéder à la page de chat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stagiaire et MDS: Le chat lié à l'utilisateur est affiché avec tout les anciens messages de la conversation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordo et Prof: Les chats lié à l'utilisateurs sont disponilbes à sélectionner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sélection un chat (coordo et prof)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le chat sélectionné est loadé et les messages du chats sont tous disponibles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chercher un chat avec la barre de recherche (coordo et prof)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seulement les chats qui contiennent le string sont encore affichés dans la sidebar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Envoyer un message</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le message est envoyé aux autres utilisateurs connectés en temps réel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Envoyer une image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L'image n'est pas envoyée</t>
+    <t>Se déconnecter</t>
+  </si>
+  <si>
+    <t>Être déconnecté</t>
+  </si>
+  <si>
+    <t>Stagiaires n'a accès qu'aux pages qui lui sont permises</t>
+  </si>
+  <si>
+    <t>Accès refusé s'il essaie d'accéder à une page à laquelle il n'a pas droit</t>
+  </si>
+  <si>
+    <t>Accès refusé avec succès</t>
+  </si>
+  <si>
+    <t>Enseignant n'a accès qu'aux pages qui lui sont permises</t>
+  </si>
+  <si>
+    <t>Maître de stage n'a accès qu'aux pages qui lui sont permises</t>
+  </si>
+  <si>
+    <t>Employeur n'a accès qu'aux pages qui lui sont permises</t>
+  </si>
+  <si>
+    <t>Coordonateur crée chaque utilisateur</t>
+  </si>
+  <si>
+    <t>Utilisateur crée</t>
+  </si>
+  <si>
+    <t>Avec succès</t>
+  </si>
+  <si>
+    <t>Coordonateur associe les utilisateurs à des rôles</t>
+  </si>
+  <si>
+    <t>Rôles associés</t>
+  </si>
+  <si>
+    <t>Coordonateur peut modifier chaque utilisateur</t>
+  </si>
+  <si>
+    <t>Utilisateur modifié</t>
+  </si>
+  <si>
+    <t>Coordonateur peut supprimer chaque utilisateur</t>
+  </si>
+  <si>
+    <t>Utilisateur supprimé</t>
+  </si>
+  <si>
+    <t>Coordonateur peut relier ensemble enseignant et stagiaire</t>
+  </si>
+  <si>
+    <t>Stagiaires-Enseignants associés</t>
+  </si>
+  <si>
+    <t>Coordonateur peut relier ensemble maître de stage s'il y a enseignant et stagiaire</t>
+  </si>
+  <si>
+    <t>Maitre de stage associés</t>
+  </si>
+  <si>
+    <t>Coordonateur peut modifier la liaison entre maître de stage et stagiaire</t>
+  </si>
+  <si>
+    <t>Liaison modifiée</t>
+  </si>
+  <si>
+    <t>Coordonateur peut modifier la liaison entre enseignant et stagiaire</t>
+  </si>
+  <si>
+    <t>Coordonateur a accès à la page de gestion des utilisateurs</t>
+  </si>
+  <si>
+    <t>Liste des utilisateurs</t>
+  </si>
+  <si>
+    <t>Coordonateur peut fournir des liens de connexion aux utilisateurs</t>
+  </si>
+  <si>
+    <t>Liens copiés</t>
+  </si>
+  <si>
+    <t>Pas encore implementé</t>
+  </si>
+  <si>
+    <t>Validation des champs de formulaires</t>
+  </si>
+  <si>
+    <t>Informations validées</t>
+  </si>
+  <si>
+    <t>Implementé, mais pas partout</t>
+  </si>
+  <si>
+    <t>Coordonateur: accéder à la page</t>
+  </si>
+  <si>
+    <t>Aucun accès</t>
+  </si>
+  <si>
+    <t>Enseignant: accéder à la page</t>
+  </si>
+  <si>
+    <t>Table de toutes les évaluations du prof est affichée</t>
+  </si>
+  <si>
+    <t>MDS et stagiaire: accéder à la page</t>
+  </si>
+  <si>
+    <t>Seulement les évaluations liées au user ET active sont affichées</t>
+  </si>
+  <si>
+    <t>Enseignant: ajouter une évaluation active</t>
+  </si>
+  <si>
+    <t>L'évaluation est créée et chaque instance est active</t>
+  </si>
+  <si>
+    <t>Enseignant: ajouter une évaluation non active</t>
+  </si>
+  <si>
+    <t>L'évaluation est créée et chaque instance n'est pas active</t>
+  </si>
+  <si>
+    <t>Enseignant: ajouter une évaluation pour les mds</t>
+  </si>
+  <si>
+    <t>Tout les mds liées aux étudiants de l'enseignant ont une évaluation créée pour eux</t>
+  </si>
+  <si>
+    <t>Enseignant: ajouter une évaluation pour les stagiaires</t>
+  </si>
+  <si>
+    <t>Tout les étudiants de l'enseignant ont une évaluation créée pour eux</t>
+  </si>
+  <si>
+    <t>Enseignant: Supprimer une évaluation</t>
+  </si>
+  <si>
+    <t>Toutes les évaluations en lien avec ce lien sont supprimées</t>
+  </si>
+  <si>
+    <t>Enseignant: changer l'activité d'une évaluation pour un utilisateur</t>
+  </si>
+  <si>
+    <t>Le nouveau status de l'évaluation est enregistré</t>
+  </si>
+  <si>
+    <t>Étudiant ou MDS: clicker sur un lien</t>
+  </si>
+  <si>
+    <t>Le status "consulté" de l'évaluation est mis à jour</t>
+  </si>
+  <si>
+    <t>Le lien est ouvert dans le browser de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Accéder à la page de chat</t>
+  </si>
+  <si>
+    <t>Stagiaire et MDS: Le chat lié à l'utilisateur est affiché avec tout les anciens messages de la conversation</t>
+  </si>
+  <si>
+    <t>Coordo et Prof: Les chats lié à l'utilisateurs sont disponilbes à sélectionner</t>
+  </si>
+  <si>
+    <t>Sélection un chat (coordo et prof)</t>
+  </si>
+  <si>
+    <t>Le chat sélectionné est loadé et les messages du chats sont tous disponibles</t>
+  </si>
+  <si>
+    <t>Chercher un chat avec la barre de recherche (coordo et prof)</t>
+  </si>
+  <si>
+    <t>Seulement les chats qui contiennent le string sont encore affichés dans la sidebar</t>
+  </si>
+  <si>
+    <t>Envoyer un message</t>
+  </si>
+  <si>
+    <t>Le message est envoyé aux autres utilisateurs connectés en temps réel</t>
+  </si>
+  <si>
+    <t>Envoyer une image</t>
+  </si>
+  <si>
+    <t>L'image n'est pas envoyée</t>
   </si>
   <si>
     <t xml:space="preserve">Envoyer un message vide </t>
   </si>
   <si>
-    <t xml:space="preserve">Le message n'est pas envoyé</t>
+    <t>Le message n'est pas envoyé</t>
+  </si>
+  <si>
+    <t>Plage horaire supprimée, retour à la page d'horaire</t>
+  </si>
+  <si>
+    <t>Retour à la page d'horaire, affichage du message d'erreur et la plage horaire n'est pas crée</t>
+  </si>
+  <si>
+    <t>Affichage de l'option d'ajout de plage horaire pour les MDS</t>
+  </si>
+  <si>
+    <t>Bouton affiché seulement pour les MDS</t>
+  </si>
+  <si>
+    <t>bouton visible et fonctionnel</t>
+  </si>
+  <si>
+    <t>Option d'ajout de plages horaire inexistant pour les stagiaires</t>
+  </si>
+  <si>
+    <t>Bouton inexistant pour les stagiaires</t>
+  </si>
+  <si>
+    <t>Échec de l'accès à la page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encore des erreurs pour les stagiaires a accédé à la plage horaire si pas d'horaire associée donc n'a pas pu être testé </t>
+  </si>
+  <si>
+    <t>Affichage de page de sélection d'horaire si MDS</t>
+  </si>
+  <si>
+    <t>Redirection a la page de sélection d'horaire</t>
+  </si>
+  <si>
+    <t>Redirige à la page de sélection d'horaire</t>
+  </si>
+  <si>
+    <t>Redirection à l'horaire associé au stagiaire s'il en a un d'associé</t>
+  </si>
+  <si>
+    <t>Redirection à la page d'horaire du stagiaire</t>
+  </si>
+  <si>
+    <t>Échec, affiche la page de sélection d'horaire</t>
+  </si>
+  <si>
+    <t>redirection en fonction du rôle n'est pas encore implémenté</t>
+  </si>
+  <si>
+    <t>Redirection du stagiaire à la page d'horaire avec un message indiquant aucun horaire si aucun ne lui est assignée</t>
+  </si>
+  <si>
+    <t>Redirection a la page d'horaire avec message "aucun horaire assigné pour le moment"</t>
+  </si>
+  <si>
+    <t>pas encore implémenté</t>
+  </si>
+  <si>
+    <t>Affichage du formulaire complet de modification de plage horaire en cliquant sur une plage horaire si MDS</t>
+  </si>
+  <si>
+    <t>Redirection vers le formulaire de modification de plage horaire</t>
+  </si>
+  <si>
+    <t>Affichage d'un pop-up demandant si on veut cocher absent ou non pour la plage horaire en cliquant sur la plage horaire si stagiaire</t>
+  </si>
+  <si>
+    <t>Affichage du pop-up swal qui demande a confirmer si on veut cocher l'absence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18.000000"/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
@@ -383,24 +466,21 @@
   </fills>
   <borders count="1">
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -412,12 +492,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -429,17 +512,23 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>4570095</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>186009</xdr:rowOff>
+      <xdr:rowOff>182199</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
@@ -469,13 +558,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
@@ -499,19 +594,25 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4046885</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>1535430</xdr:rowOff>
+      <xdr:colOff>4050695</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
@@ -535,19 +636,25 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4408462</xdr:colOff>
+      <xdr:colOff>4402747</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
@@ -565,291 +672,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1072,25 +896,27 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="C6" activeCellId="0" sqref="A2:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" width="69.77734375"/>
-    <col customWidth="1" min="2" max="2" width="43.88671875"/>
-    <col customWidth="1" min="3" max="3" width="44.33203125"/>
-    <col customWidth="1" min="4" max="4" width="75.77734375"/>
+    <col min="1" max="1" width="69.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" customWidth="1"/>
+    <col min="4" max="4" width="75.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21.75">
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1104,23 +930,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="C2" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="C3" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1128,7 +960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1136,7 +968,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1144,7 +976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" ht="121.8" customHeight="1">
+    <row r="10" spans="1:4" ht="121.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1152,7 +984,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" ht="163.19999999999999" customHeight="1">
+    <row r="11" spans="1:4" ht="163.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1160,7 +992,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" ht="121.8" customHeight="1">
+    <row r="12" spans="1:4" ht="121.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1168,7 +1000,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" ht="139.19999999999999" customHeight="1">
+    <row r="13" spans="1:4" ht="139.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1176,31 +1008,140 @@
         <v>12</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" width="69.77734375"/>
-    <col customWidth="1" min="2" max="2" width="43.88671875"/>
-    <col customWidth="1" min="3" max="3" width="44.33203125"/>
-    <col customWidth="1" min="4" max="4" width="75.77734375"/>
+    <col min="1" max="1" width="69.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" customWidth="1"/>
+    <col min="4" max="4" width="75.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21.75">
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1214,7 +1155,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1226,7 +1167,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" ht="28.5">
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -1238,7 +1179,7 @@
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1250,7 +1191,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" ht="28.5">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1264,7 +1205,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -1276,13 +1217,13 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -1294,7 +1235,7 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -1306,7 +1247,7 @@
       </c>
       <c r="D9" s="2"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -1318,7 +1259,7 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
@@ -1330,7 +1271,7 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
@@ -1342,25 +1283,25 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" ht="28.5">
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -1372,7 +1313,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" ht="28.5">
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>42</v>
       </c>
@@ -1384,7 +1325,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" ht="28.5">
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>43</v>
       </c>
@@ -1396,7 +1337,7 @@
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" ht="28.5">
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>44</v>
       </c>
@@ -1408,25 +1349,25 @@
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>45</v>
       </c>
@@ -1438,7 +1379,7 @@
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>48</v>
       </c>
@@ -1450,7 +1391,7 @@
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>50</v>
       </c>
@@ -1462,7 +1403,7 @@
       </c>
       <c r="D25" s="2"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>52</v>
       </c>
@@ -1474,13 +1415,13 @@
       </c>
       <c r="D26" s="2"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>54</v>
       </c>
@@ -1492,7 +1433,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
@@ -1504,7 +1445,7 @@
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
@@ -1516,7 +1457,7 @@
       </c>
       <c r="D30" s="2"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
@@ -1528,19 +1469,19 @@
       </c>
       <c r="D31" s="2"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>61</v>
       </c>
@@ -1552,7 +1493,7 @@
       </c>
       <c r="D34" s="2"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>63</v>
       </c>
@@ -1566,19 +1507,19 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>66</v>
       </c>
@@ -1592,250 +1533,247 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
-    <row r="54">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
-    <row r="66">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
-    <row r="67">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="65.125"/>
-    <col customWidth="1" min="2" max="2" width="73.125"/>
+    <col min="1" max="1" width="65.109375" customWidth="1"/>
+    <col min="2" max="2" width="73.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21.75">
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1849,138 +1787,113 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>79</v>
       </c>
       <c r="B7" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>81</v>
       </c>
       <c r="B8" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>83</v>
       </c>
       <c r="B9" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>85</v>
       </c>
       <c r="B10" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>87</v>
       </c>
       <c r="B11" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>87</v>
       </c>
       <c r="B12" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
     </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="54.375"/>
-    <col customWidth="1" min="2" max="2" width="79.25390625"/>
+    <col min="1" max="1" width="54.33203125" customWidth="1"/>
+    <col min="2" max="2" width="79.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21.75">
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1994,80 +1907,64 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>90</v>
       </c>
       <c r="B3" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>99</v>
       </c>
       <c r="B7" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>101</v>
       </c>
       <c r="B8" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
     </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>